<commit_message>
Mobile teams button changed
</commit_message>
<xml_diff>
--- a/src/main/resources/documents/predsjednici.xlsx
+++ b/src/main/resources/documents/predsjednici.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malin\Documents\Izbori\flow-crm-tutorial\src\main\resources\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3D1A43-D270-4B28-B632-EFD8CB06076C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872ACE81-C634-44AC-B782-4A3F47FAAEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6066,13 +6066,13 @@
     <t>065/072-903</t>
   </si>
   <si>
-    <t>DANKO</t>
-  </si>
-  <si>
     <t>1610968100013</t>
   </si>
   <si>
     <t>065/514-054</t>
+  </si>
+  <si>
+    <t>DUŠAN</t>
   </si>
 </sst>
 </file>
@@ -6913,8 +6913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A540" workbookViewId="0">
-      <selection activeCell="D550" sqref="D550"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="B178" sqref="B178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -16158,13 +16158,13 @@
         <v>285</v>
       </c>
       <c r="B550" s="8" t="s">
+        <v>2015</v>
+      </c>
+      <c r="C550" s="48" t="s">
         <v>2013</v>
       </c>
-      <c r="C550" s="48" t="s">
+      <c r="D550" s="9" t="s">
         <v>2014</v>
-      </c>
-      <c r="D550" s="9" t="s">
-        <v>2015</v>
       </c>
       <c r="E550" s="44" t="s">
         <v>1993</v>

</xml_diff>

<commit_message>
Substitutes adjusted to current state
</commit_message>
<xml_diff>
--- a/src/main/resources/documents/predsjednici.xlsx
+++ b/src/main/resources/documents/predsjednici.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malin\Documents\Izbori\flow-crm-tutorial\src\main\resources\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872ACE81-C634-44AC-B782-4A3F47FAAEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307F3EFF-FD79-4D3C-8D09-D2EE5675E9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2770" uniqueCount="2016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2769" uniqueCount="2014">
   <si>
     <t>JMBG</t>
   </si>
@@ -6066,13 +6066,7 @@
     <t>065/072-903</t>
   </si>
   <si>
-    <t>1610968100013</t>
-  </si>
-  <si>
-    <t>065/514-054</t>
-  </si>
-  <si>
-    <t>DUŠAN</t>
+    <t>1604004105009</t>
   </si>
 </sst>
 </file>
@@ -6913,8 +6907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="B178" sqref="B178"/>
+    <sheetView tabSelected="1" topLeftCell="A537" workbookViewId="0">
+      <selection activeCell="D550" sqref="D550"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8831,34 +8825,34 @@
       </c>
     </row>
     <row r="113" spans="1:5">
-      <c r="A113" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="B113" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C113" s="51" t="s">
-        <v>1526</v>
-      </c>
-      <c r="D113" s="16" t="s">
-        <v>783</v>
+      <c r="A113" s="19" t="s">
+        <v>784</v>
+      </c>
+      <c r="B113" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C113" s="53" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D113" s="20" t="s">
+        <v>785</v>
       </c>
       <c r="E113" s="15" t="s">
         <v>1966</v>
       </c>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" s="19" t="s">
-        <v>784</v>
-      </c>
-      <c r="B114" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C114" s="53" t="s">
-        <v>1527</v>
-      </c>
-      <c r="D114" s="20" t="s">
-        <v>785</v>
+      <c r="A114" s="84" t="s">
+        <v>264</v>
+      </c>
+      <c r="B114" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="C114" s="85" t="s">
+        <v>1526</v>
+      </c>
+      <c r="D114" s="84" t="s">
+        <v>783</v>
       </c>
       <c r="E114" s="18" t="s">
         <v>1969</v>
@@ -14490,34 +14484,34 @@
       </c>
     </row>
     <row r="446" spans="1:5">
-      <c r="A446" s="19" t="s">
-        <v>446</v>
-      </c>
-      <c r="B446" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C446" s="53" t="s">
-        <v>1860</v>
-      </c>
-      <c r="D446" s="20" t="s">
-        <v>1265</v>
+      <c r="A446" s="16" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B446" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C446" s="49" t="s">
+        <v>1861</v>
+      </c>
+      <c r="D446" s="12" t="s">
+        <v>1267</v>
       </c>
       <c r="E446" s="15" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="447" spans="1:5">
-      <c r="A447" s="16" t="s">
-        <v>1266</v>
-      </c>
-      <c r="B447" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C447" s="49" t="s">
-        <v>1861</v>
-      </c>
-      <c r="D447" s="12" t="s">
-        <v>1267</v>
+      <c r="A447" s="87" t="s">
+        <v>446</v>
+      </c>
+      <c r="B447" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="C447" s="88" t="s">
+        <v>1860</v>
+      </c>
+      <c r="D447" s="89" t="s">
+        <v>1265</v>
       </c>
       <c r="E447" s="18" t="s">
         <v>499</v>
@@ -16155,17 +16149,15 @@
     </row>
     <row r="550" spans="1:5">
       <c r="A550" s="8" t="s">
-        <v>285</v>
+        <v>104</v>
       </c>
       <c r="B550" s="8" t="s">
-        <v>2015</v>
+        <v>19</v>
       </c>
       <c r="C550" s="48" t="s">
         <v>2013</v>
       </c>
-      <c r="D550" s="9" t="s">
-        <v>2014</v>
-      </c>
+      <c r="D550" s="9"/>
       <c r="E550" s="44" t="s">
         <v>1993</v>
       </c>

</xml_diff>